<commit_message>
functions that need to be added to primers functions
</commit_message>
<xml_diff>
--- a/inputfiles/mockMaterials/optimal_sgRNAs_mock.xlsx
+++ b/inputfiles/mockMaterials/optimal_sgRNAs_mock.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\PycharmProjects\AutoTagsCRISPR\inputfiles\mockMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BB72564-DECC-44CA-89B7-CE25AF68B60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA24A84-E7DB-4237-9750-EAF97DBD5913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="58">
   <si>
     <t>gene_ID</t>
   </si>
@@ -188,6 +201,12 @@
   </si>
   <si>
     <t>FBtr0070244</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>sgRNA_strand</t>
   </si>
 </sst>
 </file>
@@ -219,7 +238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -242,13 +261,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -555,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +610,7 @@
     <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +653,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -661,8 +697,11 @@
       <c r="N2">
         <v>18506503</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -696,8 +735,11 @@
       <c r="N3">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -731,8 +773,11 @@
       <c r="N4">
         <v>18503976</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -766,8 +811,11 @@
       <c r="N5">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -801,8 +849,11 @@
       <c r="N6">
         <v>18478064</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -836,8 +887,11 @@
       <c r="N7">
         <v>18422621</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -871,8 +925,11 @@
       <c r="N8">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -906,8 +963,11 @@
       <c r="N9">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -941,8 +1001,11 @@
       <c r="N10">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -976,8 +1039,11 @@
       <c r="N11">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1011,8 +1077,11 @@
       <c r="N12">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1046,8 +1115,11 @@
       <c r="N13">
         <v>18422621</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1084,8 +1156,11 @@
       <c r="N14">
         <v>18515314</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1119,8 +1194,11 @@
       <c r="N15">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1154,8 +1232,11 @@
       <c r="N16">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1192,8 +1273,11 @@
       <c r="N17">
         <v>18515314</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1227,8 +1311,11 @@
       <c r="N18">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1262,8 +1349,11 @@
       <c r="N19">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1300,8 +1390,11 @@
       <c r="N20">
         <v>18515314</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1335,8 +1428,11 @@
       <c r="N21">
         <v>18422621</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1370,8 +1466,11 @@
       <c r="N22">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1405,8 +1504,11 @@
       <c r="N23">
         <v>18435756</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1440,8 +1542,11 @@
       <c r="N24">
         <v>18431427</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1478,8 +1583,11 @@
       <c r="N25">
         <v>18515314</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1513,8 +1621,11 @@
       <c r="N26">
         <v>18426128</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1548,8 +1659,12 @@
       <c r="N27">
         <v>18435756</v>
       </c>
+      <c r="O27" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>